<commit_message>
Knowledge base references polishment. Shows how knowledge representation is used a bit.
</commit_message>
<xml_diff>
--- a/backend/api/kb/Moist-to-plant.xlsx
+++ b/backend/api/kb/Moist-to-plant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KB" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="151">
   <si>
     <t>plant_type</t>
   </si>
@@ -453,14 +453,46 @@
   </si>
   <si>
     <t>81 to 100%</t>
+  </si>
+  <si>
+    <t>For row 2 to 112</t>
+  </si>
+  <si>
+    <t>Discretization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.almanac.com/plant-ph# </t>
+  </si>
+  <si>
+    <t>For row 113 to 133, however, it is pH data for the VEGATABLES, but it shows their moist levels instead as based on the previous KB website above told about the vegatables, all of them have a certain moist level.</t>
+  </si>
+  <si>
+    <t>Where it uses FOR ALL knowledge representation here.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Tahoma"/>
@@ -485,13 +517,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -793,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2274,60 +2310,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C11"/>
+  <dimension ref="B2:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>65</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>144</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C18" t="s">
         <v>145</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2" location=" "/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added life cycle plant knwoledge base and also added some data to moist level.
</commit_message>
<xml_diff>
--- a/backend/api/kb/Moist-to-plant.xlsx
+++ b/backend/api/kb/Moist-to-plant.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="172">
   <si>
     <t>plant_type</t>
   </si>
@@ -464,10 +464,73 @@
     <t xml:space="preserve">https://www.almanac.com/plant-ph# </t>
   </si>
   <si>
-    <t>For row 113 to 133, however, it is pH data for the VEGATABLES, but it shows their moist levels instead as based on the previous KB website above told about the vegatables, all of them have a certain moist level.</t>
-  </si>
-  <si>
     <t>Where it uses FOR ALL knowledge representation here.</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>Citrus</t>
+  </si>
+  <si>
+    <t>Cotton</t>
+  </si>
+  <si>
+    <t>Onion</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Sorghum</t>
+  </si>
+  <si>
+    <t>Soybean</t>
+  </si>
+  <si>
+    <t>Sugarcane</t>
+  </si>
+  <si>
+    <t>Sunflower</t>
+  </si>
+  <si>
+    <t>http://agropedia.iitk.ac.in/content/water-requirement-different-crops</t>
+  </si>
+  <si>
+    <t>Chilli</t>
+  </si>
+  <si>
+    <t>Castor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corn </t>
+  </si>
+  <si>
+    <t>Groundnut</t>
+  </si>
+  <si>
+    <t>Tobacco</t>
+  </si>
+  <si>
+    <t>Pineapple</t>
+  </si>
+  <si>
+    <t>Gingelly</t>
+  </si>
+  <si>
+    <t>Ragi</t>
+  </si>
+  <si>
+    <t>For row 113 to 132, however, it is pH data for the VEGATABLES, but it shows their moist levels instead as based on the previous KB website above told about the vegatables, all of them have a certain moist level.</t>
+  </si>
+  <si>
+    <t>Bean is removed</t>
+  </si>
+  <si>
+    <t>For row 133 to 151</t>
   </si>
 </sst>
 </file>
@@ -827,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C133"/>
+  <dimension ref="A1:C151"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A142" sqref="A142"/>
+    <sheetView topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2085,7 +2148,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B114" t="s">
         <v>5</v>
@@ -2096,7 +2159,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B115" t="s">
         <v>5</v>
@@ -2107,7 +2170,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B116" t="s">
         <v>5</v>
@@ -2118,7 +2181,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B117" t="s">
         <v>5</v>
@@ -2129,7 +2192,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B118" t="s">
         <v>5</v>
@@ -2140,7 +2203,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B119" t="s">
         <v>5</v>
@@ -2151,7 +2214,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B120" t="s">
         <v>5</v>
@@ -2162,7 +2225,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B121" t="s">
         <v>5</v>
@@ -2173,7 +2236,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B122" t="s">
         <v>5</v>
@@ -2184,7 +2247,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B123" t="s">
         <v>5</v>
@@ -2195,7 +2258,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B124" t="s">
         <v>5</v>
@@ -2206,7 +2269,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B125" t="s">
         <v>5</v>
@@ -2217,7 +2280,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B126" t="s">
         <v>5</v>
@@ -2228,7 +2291,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B127" t="s">
         <v>5</v>
@@ -2239,7 +2302,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B128" t="s">
         <v>5</v>
@@ -2250,7 +2313,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B129" t="s">
         <v>5</v>
@@ -2261,7 +2324,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B130" t="s">
         <v>5</v>
@@ -2272,7 +2335,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B131" t="s">
         <v>5</v>
@@ -2283,7 +2346,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B132" t="s">
         <v>5</v>
@@ -2294,13 +2357,211 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="B133" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C133" t="s">
-        <v>15</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>161</v>
+      </c>
+      <c r="B134" t="s">
+        <v>5</v>
+      </c>
+      <c r="C134" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>151</v>
+      </c>
+      <c r="B135" t="s">
+        <v>5</v>
+      </c>
+      <c r="C135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>159</v>
+      </c>
+      <c r="B136" t="s">
+        <v>4</v>
+      </c>
+      <c r="C136" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>156</v>
+      </c>
+      <c r="B137" t="s">
+        <v>5</v>
+      </c>
+      <c r="C137" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>162</v>
+      </c>
+      <c r="B138" t="s">
+        <v>5</v>
+      </c>
+      <c r="C138" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>163</v>
+      </c>
+      <c r="B139" t="s">
+        <v>5</v>
+      </c>
+      <c r="C139" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>118</v>
+      </c>
+      <c r="B140" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>158</v>
+      </c>
+      <c r="B141" t="s">
+        <v>15</v>
+      </c>
+      <c r="C141" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>164</v>
+      </c>
+      <c r="B142" t="s">
+        <v>5</v>
+      </c>
+      <c r="C142" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>153</v>
+      </c>
+      <c r="B143" t="s">
+        <v>15</v>
+      </c>
+      <c r="C143" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>150</v>
+      </c>
+      <c r="B144" t="s">
+        <v>15</v>
+      </c>
+      <c r="C144" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>157</v>
+      </c>
+      <c r="B145" t="s">
+        <v>5</v>
+      </c>
+      <c r="C145" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>152</v>
+      </c>
+      <c r="B146" t="s">
+        <v>15</v>
+      </c>
+      <c r="C146" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>165</v>
+      </c>
+      <c r="B147" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>166</v>
+      </c>
+      <c r="B148" t="s">
+        <v>15</v>
+      </c>
+      <c r="C148" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>167</v>
+      </c>
+      <c r="B149" t="s">
+        <v>4</v>
+      </c>
+      <c r="C149" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>168</v>
+      </c>
+      <c r="B150" t="s">
+        <v>5</v>
+      </c>
+      <c r="C150" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>154</v>
+      </c>
+      <c r="B151" t="s">
+        <v>4</v>
+      </c>
+      <c r="C151" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2310,45 +2571,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E18"/>
+  <dimension ref="B2:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="K7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>65</v>
       </c>
@@ -2356,7 +2630,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>4</v>
       </c>
@@ -2364,7 +2638,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>5</v>
       </c>

</xml_diff>